<commit_message>
added card multiples to sample-game.xlsx
</commit_message>
<xml_diff>
--- a/workbooks/sample-game.xlsx
+++ b/workbooks/sample-game.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11480" yWindow="2420" windowWidth="21680" windowHeight="14240" tabRatio="656" activeTab="1"/>
+    <workbookView xWindow="7120" yWindow="2420" windowWidth="21680" windowHeight="14240" tabRatio="656"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Game" sheetId="19" r:id="rId1"/>
@@ -2440,8 +2440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2797,7 +2797,7 @@
     </row>
     <row r="20" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>152</v>
@@ -2849,7 +2849,7 @@
     </row>
     <row r="21" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>219</v>
@@ -2901,7 +2901,7 @@
     </row>
     <row r="22" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="25" t="s">
         <v>147</v>
@@ -2963,7 +2963,7 @@
     </row>
     <row r="23" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="46">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>148</v>
@@ -3081,7 +3081,7 @@
     </row>
     <row r="25" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>184</v>
@@ -3322,7 +3322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>